<commit_message>
Application has been completed
</commit_message>
<xml_diff>
--- a/DesignTable1.xlsx
+++ b/DesignTable1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasho\Desktop\CatiaScripts\Group-dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDF5089-2BC3-4780-B661-32E203B6572B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38684202-880E-4BBB-BB05-C1CAF786D7E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AD0A256B-BABC-48BD-B036-8BF40D88CEF9}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>